<commit_message>
update lyrics and album covers
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtroelfs/Dropbox/Personal/scripts/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52E7FB-8FA1-7C4D-BB12-5F7F28F3E38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA7445-0EFC-9041-9F23-B14C28C92951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="130">
   <si>
     <t>album_name</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>Speak Now (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>1989 (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>1989 (Taylor's Version) [Deluxe]</t>
   </si>
 </sst>
 </file>
@@ -1252,11 +1258,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2564,6 +2570,22 @@
         <v>45114</v>
       </c>
     </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>128</v>
+      </c>
+      <c r="D132" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>129</v>
+      </c>
+      <c r="D133" s="1">
+        <v>45226</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>